<commit_message>
Update examples and documentation
</commit_message>
<xml_diff>
--- a/Harris_County/Documentation/Harris_County_2018_bg_config.xlsx
+++ b/Harris_County/Documentation/Harris_County_2018_bg_config.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['QEXTRCT' 'QNOHLTH' 'QPOVTY' 'QHISPC' 'QESL' 'PPUNIT' 'QEDLESHI' 'PERCAP']</t>
+          <t>['QEDLESHI' 'PPUNIT' 'QHISPC' 'QEXTRCT' 'QESL' 'QNOHLTH' 'QPOVTY' 'PERCAP']</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['QPOVTY' 'QFAM' 'QFHH' 'QSERV' 'QBLACK' 'PERCAP' 'QRICH']</t>
+          <t>['QPOVTY' 'QSERV' 'QFHH' 'QBLACK' 'QFAM' 'PERCAP' 'QRICH']</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['QAGEDEP' 'QFEMLBR' 'QFEMALE']</t>
+          <t>['QAGEDEP' 'QFEMALE' 'QFEMLBR']</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['QRENTER' 'QAGEDEP' 'QSSBEN' 'MEDAGE']</t>
+          <t>['QRENTER' 'QAGEDEP' 'MEDAGE' 'QSSBEN']</t>
         </is>
       </c>
     </row>
@@ -583,89 +583,89 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>QEXTRCT</t>
+          <t>QEDLESHI</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7518642495108142</v>
+        <v>0.8692554782357783</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1080633728002054</v>
+        <v>0.2820098258644139</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1841536346678236</v>
+        <v>-0.09611805589828241</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.04880562735300907</v>
+        <v>-0.04435359344350712</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02811185885597966</v>
+        <v>0.01766608403865631</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>QNOHLTH</t>
+          <t>PPUNIT</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7427426222143544</v>
+        <v>0.5203431740155542</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3825258293668706</v>
+        <v>0.1723556441346736</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.09377154755937264</v>
+        <v>-0.008531185261721667</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.1242320388317747</v>
+        <v>-0.04118569706715453</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1047037157728299</v>
+        <v>-0.6351977716203236</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>QPOVTY</t>
+          <t>QHISPC</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4926703476287158</v>
+        <v>0.8803370957544391</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4936970992516587</v>
+        <v>0.1202941239550452</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01006171224206333</v>
+        <v>-0.1034740118703461</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1399809112142014</v>
+        <v>-0.2055870767799969</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3593031995970374</v>
+        <v>-0.1433395973189483</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>QHISPC</t>
+          <t>QEXTRCT</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8803370990651693</v>
+        <v>0.7518642473093413</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1202941224184667</v>
+        <v>0.1080633735595425</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.1034740109136102</v>
+        <v>-0.1841536326290315</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.2055870782703638</v>
+        <v>-0.04880562998113309</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.143339598722074</v>
+        <v>0.02811185768577718</v>
       </c>
     </row>
     <row r="6">
@@ -675,85 +675,85 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8669870514215789</v>
+        <v>0.866987049019839</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1055887569373343</v>
+        <v>0.1055887591660848</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1218582045111581</v>
+        <v>-0.1218582046621672</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1645406172047933</v>
+        <v>-0.1645406170571051</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1246202492925805</v>
+        <v>0.124620247327293</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>PPUNIT</t>
+          <t>QNOHLTH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5203431742265832</v>
+        <v>0.7427426207000754</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1723556460387186</v>
+        <v>0.3825258297491037</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.00853118525952266</v>
+        <v>-0.09377154715997181</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.04118569695642556</v>
+        <v>-0.1242320393971812</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.6351977724633163</v>
+        <v>0.1047037140321911</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>QEDLESHI</t>
+          <t>QPOVTY</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8692554807126757</v>
+        <v>0.4926703471130989</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2820098255090495</v>
+        <v>0.4936971007074465</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.09611805627276045</v>
+        <v>0.01006171172543471</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.04435359216347973</v>
+        <v>-0.1399809107396388</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01766608473076514</v>
+        <v>0.3593031970426002</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>QFAM</t>
+          <t>QSERV</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1243576369004263</v>
+        <v>0.3709861026223996</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6629400831629817</v>
+        <v>0.5379072882887543</v>
       </c>
       <c r="D9" t="n">
-        <v>0.07601970060271199</v>
+        <v>0.00575919881979431</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.1184125639975566</v>
+        <v>-0.0875776964683645</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2379119010605504</v>
+        <v>0.1559839714259979</v>
       </c>
     </row>
     <row r="10">
@@ -763,63 +763,63 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2285252631954916</v>
+        <v>0.2285252628627771</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7131346625644719</v>
+        <v>0.7131346598683198</v>
       </c>
       <c r="D10" t="n">
-        <v>0.221464652827946</v>
+        <v>0.2214646500776639</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0778327826040513</v>
+        <v>-0.07783278026777046</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.04601151927811519</v>
+        <v>-0.04601151877673739</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>QSERV</t>
+          <t>QBLACK</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3709861031127151</v>
+        <v>-0.2749361524699589</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5379072879847436</v>
+        <v>0.704648556134802</v>
       </c>
       <c r="D11" t="n">
-        <v>0.005759199147247418</v>
+        <v>0.05019711367311201</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.08757769675265198</v>
+        <v>0.1307361797650962</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1559839732810449</v>
+        <v>0.1670202060833451</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>QBLACK</t>
+          <t>QFAM</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.2749361547003947</v>
+        <v>0.1243576373666156</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7046485612883941</v>
+        <v>0.6629400806657814</v>
       </c>
       <c r="D12" t="n">
-        <v>0.05019711150284902</v>
+        <v>0.07601969973533645</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1307361829377608</v>
+        <v>-0.118412562716169</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1670202081525151</v>
+        <v>0.2379118982834663</v>
       </c>
     </row>
     <row r="13">
@@ -829,19 +829,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5037823285394682</v>
+        <v>0.5037823274519664</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7061433380601022</v>
+        <v>0.706143335809101</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.04688443612431405</v>
+        <v>-0.04688443578342617</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1072480908368672</v>
+        <v>-0.1072480917650937</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.1020625157575887</v>
+        <v>-0.1020625160227645</v>
       </c>
     </row>
     <row r="14">
@@ -851,19 +851,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.403877885318759</v>
+        <v>0.403877884430713</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6463639823681145</v>
+        <v>0.6463639841834479</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.06158260902562788</v>
+        <v>-0.06158260947039726</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.1194534709466674</v>
+        <v>-0.1194534714731934</v>
       </c>
       <c r="F14" t="n">
-        <v>0.002273123311216117</v>
+        <v>0.002273120718433929</v>
       </c>
     </row>
     <row r="15">
@@ -873,19 +873,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.189130410850255</v>
+        <v>0.189130410502966</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3968119673856886</v>
+        <v>0.3968119687604864</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.001312813336785004</v>
+        <v>-0.001312813302421819</v>
       </c>
       <c r="E15" t="n">
-        <v>0.08291571237027733</v>
+        <v>0.08291571109167226</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5521493372662168</v>
+        <v>0.5521493329099174</v>
       </c>
     </row>
     <row r="16">
@@ -895,19 +895,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.172722742608773</v>
+        <v>0.17272274185355</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3584593750335594</v>
+        <v>0.3584593782385577</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.0564280904172438</v>
+        <v>-0.05642809085152523</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.4605499135181512</v>
+        <v>-0.4605499124871737</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6579699997974613</v>
+        <v>0.657969995084253</v>
       </c>
     </row>
     <row r="17">
@@ -917,107 +917,107 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.1133192029759045</v>
+        <v>-0.1133192111059629</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.06739481490009445</v>
+        <v>-0.0673948075316152</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7290404243689187</v>
+        <v>0.7290403985390425</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4777003088360845</v>
+        <v>0.4777003030203259</v>
       </c>
       <c r="F17" t="n">
-        <v>0.06612984172625579</v>
+        <v>0.06612983556966748</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>QFEMLBR</t>
+          <t>QFEMALE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.4233895411224217</v>
+        <v>-0.1201784064898982</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2565876932114498</v>
+        <v>0.08442001436012979</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5549136275201361</v>
+        <v>0.9476421078584786</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.009510220414830017</v>
+        <v>0.01306748466847658</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.03382139000588</v>
+        <v>-0.03709586634662605</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>QFEMALE</t>
+          <t>QFEMLBR</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.1201784094880135</v>
+        <v>-0.4233895396708394</v>
       </c>
       <c r="C19" t="n">
-        <v>0.08442001645054158</v>
+        <v>0.2565876918738777</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9476420897190044</v>
+        <v>0.5549136198598398</v>
       </c>
       <c r="E19" t="n">
-        <v>0.01306748272590304</v>
+        <v>-0.009510213121744099</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.0370958680276902</v>
+        <v>-0.03382138775670606</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>QSSBEN</t>
+          <t>MEDAGE</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.08069646320798909</v>
+        <v>-0.3065470996556154</v>
       </c>
       <c r="C20" t="n">
-        <v>0.07089796289656143</v>
+        <v>-0.3702019272504437</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1345297522283367</v>
+        <v>0.04864970456986826</v>
       </c>
       <c r="E20" t="n">
-        <v>0.847625127427726</v>
+        <v>0.6451312876761621</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.1136918287074245</v>
+        <v>0.09075703990682774</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>MEDAGE</t>
+          <t>QSSBEN</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.3065471006736213</v>
+        <v>-0.08069646329989939</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.3702019263708303</v>
+        <v>0.07089796186361795</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0486497043881483</v>
+        <v>0.1345297509011206</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6451312883412534</v>
+        <v>0.8476251258068529</v>
       </c>
       <c r="F21" t="n">
-        <v>0.09075703809612549</v>
+        <v>-0.1136918281150361</v>
       </c>
     </row>
   </sheetData>
@@ -1108,40 +1108,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.794886792638567</v>
+        <v>4.794886974007128</v>
       </c>
       <c r="C2" t="n">
-        <v>2.924553801425152</v>
+        <v>2.924553900504404</v>
       </c>
       <c r="D2" t="n">
-        <v>2.224021662842042</v>
+        <v>2.22402164593982</v>
       </c>
       <c r="E2" t="n">
-        <v>1.964387329553392</v>
+        <v>1.964387356238504</v>
       </c>
       <c r="F2" t="n">
-        <v>1.939969527478589</v>
+        <v>1.939969486264947</v>
       </c>
       <c r="G2" t="n">
-        <v>1.919869560350441</v>
+        <v>1.919869526961092</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6695953046457972</v>
+        <v>0.6695949908256502</v>
       </c>
       <c r="I2" t="n">
-        <v>4.983165063082106</v>
+        <v>4.983165037946606</v>
       </c>
       <c r="J2" t="n">
-        <v>3.692480351167769</v>
+        <v>3.69248034038259</v>
       </c>
       <c r="K2" t="n">
-        <v>1.902149236363422</v>
+        <v>1.902149222502244</v>
       </c>
       <c r="L2" t="n">
-        <v>1.76312873554119</v>
+        <v>1.763128723633083</v>
       </c>
       <c r="M2" t="n">
-        <v>1.467933717339212</v>
+        <v>1.4679336985806</v>
       </c>
     </row>
     <row r="3">
@@ -1151,40 +1151,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1775883997273544</v>
+        <v>0.1775884064447084</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1083168074601908</v>
+        <v>0.1083168111297927</v>
       </c>
       <c r="D3" t="n">
-        <v>0.08237117269785339</v>
+        <v>0.0823711720718452</v>
       </c>
       <c r="E3" t="n">
-        <v>0.07275508627975526</v>
+        <v>0.07275508726809274</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07185072323994775</v>
+        <v>0.07185072171351656</v>
       </c>
       <c r="G3" t="n">
-        <v>0.07110628001297931</v>
+        <v>0.07110627877633673</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02479982609799249</v>
+        <v>0.02479981447502408</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2491582531541053</v>
+        <v>0.2491582518973303</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1846240175583885</v>
+        <v>0.1846240170191295</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09510746181817108</v>
+        <v>0.09510746112511219</v>
       </c>
       <c r="L3" t="n">
-        <v>0.08815643677705949</v>
+        <v>0.08815643618165415</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0733966858669606</v>
+        <v>0.07339668492903</v>
       </c>
     </row>
     <row r="4">
@@ -1194,40 +1194,40 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1775883997273544</v>
+        <v>0.1775884064447084</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2859052071875452</v>
+        <v>0.2859052175745012</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3682763798853986</v>
+        <v>0.3682763896463463</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4410314661651538</v>
+        <v>0.4410314769144391</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5128821894051016</v>
+        <v>0.5128821986279557</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5839884694180808</v>
+        <v>0.5839884774042924</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6087882955160733</v>
+        <v>0.6087882918793165</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2491582531541053</v>
+        <v>0.2491582518973303</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4337822707124938</v>
+        <v>0.4337822689164598</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5288897325306648</v>
+        <v>0.528889730041572</v>
       </c>
       <c r="L4" t="n">
-        <v>0.6170461693077244</v>
+        <v>0.6170461662232262</v>
       </c>
       <c r="M4" t="n">
-        <v>0.690442855174685</v>
+        <v>0.6904428511522561</v>
       </c>
     </row>
     <row r="5">
@@ -1237,40 +1237,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2917079730923731</v>
+        <v>0.2917079858689411</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1779219611447524</v>
+        <v>0.1779219682353303</v>
       </c>
       <c r="D5" t="n">
-        <v>0.135303476273352</v>
+        <v>0.1353034760533373</v>
       </c>
       <c r="E5" t="n">
-        <v>0.11950802407934</v>
+        <v>0.1195080264167028</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1180225108944308</v>
+        <v>0.1180225090921425</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1167996831356656</v>
+        <v>0.1167996818020812</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0407363713800863</v>
+        <v>0.04073635253146473</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3608673060872897</v>
+        <v>0.3608673063694102</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2673994178876365</v>
+        <v>0.2673994186644367</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1377484915737284</v>
+        <v>0.137748491372444</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1276810037446988</v>
+        <v>0.1276810036261987</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1063037807066465</v>
+        <v>0.1063037799675104</v>
       </c>
     </row>
   </sheetData>
@@ -1326,19 +1326,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.983165063082106</v>
+        <v>4.983165037946606</v>
       </c>
       <c r="C2" t="n">
-        <v>3.692480351167769</v>
+        <v>3.69248034038259</v>
       </c>
       <c r="D2" t="n">
-        <v>1.902149236363422</v>
+        <v>1.902149222502244</v>
       </c>
       <c r="E2" t="n">
-        <v>1.76312873554119</v>
+        <v>1.763128723633083</v>
       </c>
       <c r="F2" t="n">
-        <v>1.467933717339212</v>
+        <v>1.4679336985806</v>
       </c>
     </row>
     <row r="3">
@@ -1348,19 +1348,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2491582531541053</v>
+        <v>0.2491582518973303</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1846240175583885</v>
+        <v>0.1846240170191295</v>
       </c>
       <c r="D3" t="n">
-        <v>0.09510746181817108</v>
+        <v>0.09510746112511219</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08815643677705949</v>
+        <v>0.08815643618165415</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0733966858669606</v>
+        <v>0.07339668492903</v>
       </c>
     </row>
     <row r="4">
@@ -1370,19 +1370,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2491582531541053</v>
+        <v>0.2491582518973303</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4337822707124938</v>
+        <v>0.4337822689164598</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5288897325306648</v>
+        <v>0.528889730041572</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6170461693077244</v>
+        <v>0.6170461662232262</v>
       </c>
       <c r="F4" t="n">
-        <v>0.690442855174685</v>
+        <v>0.6904428511522561</v>
       </c>
     </row>
     <row r="5">
@@ -1392,19 +1392,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3608673060872897</v>
+        <v>0.3608673063694102</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2673994178876365</v>
+        <v>0.2673994186644367</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1377484915737284</v>
+        <v>0.137748491372444</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1276810037446988</v>
+        <v>0.1276810036261987</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1063037807066465</v>
+        <v>0.1063037799675104</v>
       </c>
     </row>
   </sheetData>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[['QEXTRCT', 'QNOHLTH', 'QPOVTY', 'QHISPC', 'QESL', 'PPUNIT', 'QEDLESHI', 'PERCAP', 'QFAM', 'QFHH', 'QSERV', 'QBLACK', 'QRICH', 'QAGEDEP', 'QFEMLBR', 'QFEMALE', 'QRENTER', 'QSSBEN', 'MEDAGE', 'QNOAUTO']]</t>
+          <t>[['QEDLESHI', 'PPUNIT', 'QHISPC', 'QEXTRCT', 'QESL', 'QNOHLTH', 'QPOVTY', 'PERCAP', 'QSERV', 'QFHH', 'QBLACK', 'QFAM', 'QRICH', 'QAGEDEP', 'QFEMALE', 'QFEMLBR', 'QRENTER', 'MEDAGE', 'QSSBEN', 'QNOAUTO']]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">

</xml_diff>

<commit_message>
final test run of Harris County
</commit_message>
<xml_diff>
--- a/Harris_County/Documentation/Harris_County_2018_bg_config.xlsx
+++ b/Harris_County/Documentation/Harris_County_2018_bg_config.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['QEDLESHI' 'PPUNIT' 'QHISPC' 'QEXTRCT' 'QESL' 'QNOHLTH' 'QPOVTY' 'PERCAP']</t>
+          <t>['QEXTRCT' 'QEDLESHI' 'QNOHLTH' 'QPOVTY' 'QESL' 'QHISPC' 'PPUNIT' 'PERCAP']</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['QPOVTY' 'QSERV' 'QFHH' 'QBLACK' 'QFAM' 'PERCAP' 'QRICH']</t>
+          <t>['QPOVTY' 'QFAM' 'QFHH' 'QBLACK' 'QSERV' 'PERCAP' 'QRICH']</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['QAGEDEP' 'QFEMALE' 'QFEMLBR']</t>
+          <t>['QFEMLBR' 'QFEMALE' 'QAGEDEP']</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['PPUNIT' 'QNOAUTO' 'QRENTER']</t>
+          <t>['PPUNIT' 'QRENTER' 'QNOAUTO']</t>
         </is>
       </c>
     </row>
@@ -583,89 +583,89 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>QEDLESHI</t>
+          <t>QEXTRCT</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8692554782357783</v>
+        <v>0.7518642484417047</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2820098258644139</v>
+        <v>0.1080633726986945</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.09611805589828241</v>
+        <v>-0.184153634128851</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.04435359344350712</v>
+        <v>-0.04880562950779412</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01766608403865631</v>
+        <v>0.02811185968668175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>PPUNIT</t>
+          <t>QEDLESHI</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5203431740155542</v>
+        <v>0.8692554802113335</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1723556441346736</v>
+        <v>0.2820098251129958</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.008531185261721667</v>
+        <v>-0.09611805635391178</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.04118569706715453</v>
+        <v>-0.04435359362502852</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.6351977716203236</v>
+        <v>0.01766608572966158</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>QHISPC</t>
+          <t>QNOHLTH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8803370957544391</v>
+        <v>0.7427426205749446</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1202941239550452</v>
+        <v>0.3825258292209991</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.1034740118703461</v>
+        <v>-0.09377154783409625</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.2055870767799969</v>
+        <v>-0.1242320404236909</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1433395973189483</v>
+        <v>0.1047037153226807</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>QEXTRCT</t>
+          <t>QPOVTY</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7518642473093413</v>
+        <v>0.4926703472929525</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1080633735595425</v>
+        <v>0.4936971001788416</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.1841536326290315</v>
+        <v>0.01006171257136397</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.04880562998113309</v>
+        <v>-0.139980912263577</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02811185768577718</v>
+        <v>0.359303199780186</v>
       </c>
     </row>
     <row r="6">
@@ -675,85 +675,85 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.866987049019839</v>
+        <v>0.8669870460373705</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1055887591660848</v>
+        <v>0.105588759382269</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1218582046621672</v>
+        <v>-0.1218582062889729</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1645406170571051</v>
+        <v>-0.1645406179565412</v>
       </c>
       <c r="F6" t="n">
-        <v>0.124620247327293</v>
+        <v>0.1246202480462146</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>QNOHLTH</t>
+          <t>QHISPC</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7427426207000754</v>
+        <v>0.8803370942915406</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3825258297491037</v>
+        <v>0.1202941229291331</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.09377154715997181</v>
+        <v>-0.1034740124261152</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1242320393971812</v>
+        <v>-0.205587078981756</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1047037140321911</v>
+        <v>-0.1433395948207157</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>QPOVTY</t>
+          <t>PPUNIT</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4926703471130989</v>
+        <v>0.5203431752795143</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4936971007074465</v>
+        <v>0.1723556415683452</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01006171172543471</v>
+        <v>-0.008531183769641909</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1399809107396388</v>
+        <v>-0.0411856994804425</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3593031970426002</v>
+        <v>-0.6351977636422353</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>QSERV</t>
+          <t>QFAM</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.3709861026223996</v>
+        <v>0.1243576377146733</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5379072882887543</v>
+        <v>0.66294007956358</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00575919881979431</v>
+        <v>0.07601970061597395</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0875776964683645</v>
+        <v>-0.1184125638687395</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1559839714259979</v>
+        <v>0.2379118979678956</v>
       </c>
     </row>
     <row r="10">
@@ -763,19 +763,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2285252628627771</v>
+        <v>0.2285252645071095</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7131346598683198</v>
+        <v>0.7131346566768045</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2214646500776639</v>
+        <v>0.2214646517180176</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.07783278026777046</v>
+        <v>-0.07783278306666057</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.04601151877673739</v>
+        <v>-0.04601151712576505</v>
       </c>
     </row>
     <row r="11">
@@ -785,41 +785,41 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.2749361524699589</v>
+        <v>-0.2749361517443922</v>
       </c>
       <c r="C11" t="n">
-        <v>0.704648556134802</v>
+        <v>0.7046485571608363</v>
       </c>
       <c r="D11" t="n">
-        <v>0.05019711367311201</v>
+        <v>0.05019711414732955</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1307361797650962</v>
+        <v>0.1307361802183043</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1670202060833451</v>
+        <v>0.1670202047959224</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>QFAM</t>
+          <t>QSERV</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1243576373666156</v>
+        <v>0.3709861023078258</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6629400806657814</v>
+        <v>0.5379072869833532</v>
       </c>
       <c r="D12" t="n">
-        <v>0.07601969973533645</v>
+        <v>0.005759199128988558</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.118412562716169</v>
+        <v>-0.08757769803385232</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2379118982834663</v>
+        <v>0.1559839714480021</v>
       </c>
     </row>
     <row r="13">
@@ -829,19 +829,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5037823274519664</v>
+        <v>0.5037823282541694</v>
       </c>
       <c r="C13" t="n">
-        <v>0.706143335809101</v>
+        <v>0.7061433337952319</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.04688443578342617</v>
+        <v>-0.04688443481784117</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1072480917650937</v>
+        <v>-0.1072480938194731</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.1020625160227645</v>
+        <v>-0.1020625141790412</v>
       </c>
     </row>
     <row r="14">
@@ -851,85 +851,85 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.403877884430713</v>
+        <v>0.4038778847879076</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6463639841834479</v>
+        <v>0.6463639839109264</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.06158260947039726</v>
+        <v>-0.06158260922857307</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.1194534714731934</v>
+        <v>-0.1194534731552246</v>
       </c>
       <c r="F14" t="n">
-        <v>0.002273120718433929</v>
+        <v>0.002273121035538215</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>QNOAUTO</t>
+          <t>QRENTER</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.189130410502966</v>
+        <v>0.1727227398097679</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3968119687604864</v>
+        <v>0.3584593755415023</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.001312813302421819</v>
+        <v>-0.05642808994004768</v>
       </c>
       <c r="E15" t="n">
-        <v>0.08291571109167226</v>
+        <v>-0.4605499177939512</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5521493329099174</v>
+        <v>0.6579700024315055</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>QRENTER</t>
+          <t>QNOAUTO</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.17272274185355</v>
+        <v>0.1891304089967761</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3584593782385577</v>
+        <v>0.3968119693850521</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.05642809085152523</v>
+        <v>-0.001312813646046432</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.4605499124871737</v>
+        <v>0.0829157104879002</v>
       </c>
       <c r="F16" t="n">
-        <v>0.657969995084253</v>
+        <v>0.5521493306898304</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>QAGEDEP</t>
+          <t>QFEMLBR</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.1133192111059629</v>
+        <v>-0.4233895386433378</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.0673948075316152</v>
+        <v>0.2565876909270864</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7290403985390425</v>
+        <v>0.5549136206110808</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4777003030203259</v>
+        <v>-0.009510215744995571</v>
       </c>
       <c r="F17" t="n">
-        <v>0.06612983556966748</v>
+        <v>-0.03382138915842849</v>
       </c>
     </row>
     <row r="18">
@@ -939,41 +939,41 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.1201784064898982</v>
+        <v>-0.1201784102251344</v>
       </c>
       <c r="C18" t="n">
-        <v>0.08442001436012979</v>
+        <v>0.08442001701203185</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9476421078584786</v>
+        <v>0.9476420859302027</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01306748466847658</v>
+        <v>0.01306748493548795</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.03709586634662605</v>
+        <v>-0.03709586765110615</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>QFEMLBR</t>
+          <t>QAGEDEP</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.4233895396708394</v>
+        <v>-0.1133192053356318</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2565876918738777</v>
+        <v>-0.06739481110732691</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5549136198598398</v>
+        <v>0.7290404171908992</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.009510213121744099</v>
+        <v>0.4777003064674182</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.03382138775670606</v>
+        <v>0.06612983910678825</v>
       </c>
     </row>
     <row r="20">
@@ -983,19 +983,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.3065470996556154</v>
+        <v>-0.3065470993356068</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.3702019272504437</v>
+        <v>-0.3702019246123122</v>
       </c>
       <c r="D20" t="n">
-        <v>0.04864970456986826</v>
+        <v>0.04864970172662886</v>
       </c>
       <c r="E20" t="n">
-        <v>0.6451312876761621</v>
+        <v>0.6451312986528182</v>
       </c>
       <c r="F20" t="n">
-        <v>0.09075703990682774</v>
+        <v>0.09075704017158054</v>
       </c>
     </row>
     <row r="21">
@@ -1005,19 +1005,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.08069646329989939</v>
+        <v>-0.08069646398190604</v>
       </c>
       <c r="C21" t="n">
-        <v>0.07089796186361795</v>
+        <v>0.07089796134946129</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1345297509011206</v>
+        <v>0.1345297551567557</v>
       </c>
       <c r="E21" t="n">
-        <v>0.8476251258068529</v>
+        <v>0.8476251059191149</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.1136918281150361</v>
+        <v>-0.1136918292190382</v>
       </c>
     </row>
   </sheetData>
@@ -1129,19 +1129,19 @@
         <v>0.6695949908256502</v>
       </c>
       <c r="I2" t="n">
-        <v>4.983165037946606</v>
+        <v>4.983165035304014</v>
       </c>
       <c r="J2" t="n">
-        <v>3.69248034038259</v>
+        <v>3.692480325572514</v>
       </c>
       <c r="K2" t="n">
-        <v>1.902149222502244</v>
+        <v>1.902149211798767</v>
       </c>
       <c r="L2" t="n">
-        <v>1.763128723633083</v>
+        <v>1.763128716214867</v>
       </c>
       <c r="M2" t="n">
-        <v>1.4679336985806</v>
+        <v>1.467933697393225</v>
       </c>
     </row>
     <row r="3">
@@ -1172,19 +1172,19 @@
         <v>0.02479981447502408</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2491582518973303</v>
+        <v>0.2491582517652007</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1846240170191295</v>
+        <v>0.1846240162786257</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09510746112511219</v>
+        <v>0.09510746058993837</v>
       </c>
       <c r="L3" t="n">
-        <v>0.08815643618165415</v>
+        <v>0.08815643581074337</v>
       </c>
       <c r="M3" t="n">
-        <v>0.07339668492903</v>
+        <v>0.07339668486966126</v>
       </c>
     </row>
     <row r="4">
@@ -1215,19 +1215,19 @@
         <v>0.6087882918793165</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2491582518973303</v>
+        <v>0.2491582517652007</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4337822689164598</v>
+        <v>0.4337822680438264</v>
       </c>
       <c r="K4" t="n">
-        <v>0.528889730041572</v>
+        <v>0.5288897286337648</v>
       </c>
       <c r="L4" t="n">
-        <v>0.6170461662232262</v>
+        <v>0.6170461644445082</v>
       </c>
       <c r="M4" t="n">
-        <v>0.6904428511522561</v>
+        <v>0.6904428493141694</v>
       </c>
     </row>
     <row r="5">
@@ -1258,19 +1258,19 @@
         <v>0.04073635253146473</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3608673063694102</v>
+        <v>0.3608673071387364</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2673994186644367</v>
+        <v>0.267399418303798</v>
       </c>
       <c r="K5" t="n">
-        <v>0.137748491372444</v>
+        <v>0.1377484909640392</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1276810036261987</v>
+        <v>0.127681003428902</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1063037799675104</v>
+        <v>0.1063037801645243</v>
       </c>
     </row>
   </sheetData>
@@ -1326,19 +1326,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.983165037946606</v>
+        <v>4.983165035304014</v>
       </c>
       <c r="C2" t="n">
-        <v>3.69248034038259</v>
+        <v>3.692480325572514</v>
       </c>
       <c r="D2" t="n">
-        <v>1.902149222502244</v>
+        <v>1.902149211798767</v>
       </c>
       <c r="E2" t="n">
-        <v>1.763128723633083</v>
+        <v>1.763128716214867</v>
       </c>
       <c r="F2" t="n">
-        <v>1.4679336985806</v>
+        <v>1.467933697393225</v>
       </c>
     </row>
     <row r="3">
@@ -1348,19 +1348,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2491582518973303</v>
+        <v>0.2491582517652007</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1846240170191295</v>
+        <v>0.1846240162786257</v>
       </c>
       <c r="D3" t="n">
-        <v>0.09510746112511219</v>
+        <v>0.09510746058993837</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08815643618165415</v>
+        <v>0.08815643581074337</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07339668492903</v>
+        <v>0.07339668486966126</v>
       </c>
     </row>
     <row r="4">
@@ -1370,19 +1370,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2491582518973303</v>
+        <v>0.2491582517652007</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4337822689164598</v>
+        <v>0.4337822680438264</v>
       </c>
       <c r="D4" t="n">
-        <v>0.528889730041572</v>
+        <v>0.5288897286337648</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6170461662232262</v>
+        <v>0.6170461644445082</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6904428511522561</v>
+        <v>0.6904428493141694</v>
       </c>
     </row>
     <row r="5">
@@ -1392,19 +1392,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3608673063694102</v>
+        <v>0.3608673071387364</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2673994186644367</v>
+        <v>0.267399418303798</v>
       </c>
       <c r="D5" t="n">
-        <v>0.137748491372444</v>
+        <v>0.1377484909640392</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1276810036261987</v>
+        <v>0.127681003428902</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1063037799675104</v>
+        <v>0.1063037801645243</v>
       </c>
     </row>
   </sheetData>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[['QEDLESHI', 'PPUNIT', 'QHISPC', 'QEXTRCT', 'QESL', 'QNOHLTH', 'QPOVTY', 'PERCAP', 'QSERV', 'QFHH', 'QBLACK', 'QFAM', 'QRICH', 'QAGEDEP', 'QFEMALE', 'QFEMLBR', 'QRENTER', 'MEDAGE', 'QSSBEN', 'QNOAUTO']]</t>
+          <t>[['QEXTRCT', 'QEDLESHI', 'QNOHLTH', 'QPOVTY', 'QESL', 'QHISPC', 'PPUNIT', 'PERCAP', 'QFAM', 'QFHH', 'QBLACK', 'QSERV', 'QRICH', 'QFEMLBR', 'QFEMALE', 'QAGEDEP', 'QRENTER', 'MEDAGE', 'QSSBEN', 'QNOAUTO']]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">

</xml_diff>

<commit_message>
updates to examples and data license
</commit_message>
<xml_diff>
--- a/Harris_County/Documentation/Harris_County_2018_bg_config.xlsx
+++ b/Harris_County/Documentation/Harris_County_2018_bg_config.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['QEXTRCT' 'QEDLESHI' 'QNOHLTH' 'QPOVTY' 'QESL' 'QHISPC' 'PPUNIT' 'PERCAP']</t>
+          <t>['QHISPC' 'QNOHLTH' 'QESL' 'QEXTRCT' 'QEDLESHI' 'PPUNIT' 'QPOVTY' 'PERCAP']</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['QPOVTY' 'QFAM' 'QFHH' 'QBLACK' 'QSERV' 'PERCAP' 'QRICH']</t>
+          <t>['QPOVTY' 'QFAM' 'QSERV' 'QFHH' 'QBLACK' 'QRICH' 'PERCAP']</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['QFEMLBR' 'QFEMALE' 'QAGEDEP']</t>
+          <t>['QFEMALE' 'QFEMLBR' 'QAGEDEP']</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['PPUNIT' 'QRENTER' 'QNOAUTO']</t>
+          <t>['PPUNIT' 'QNOAUTO' 'QRENTER']</t>
         </is>
       </c>
     </row>
@@ -583,155 +583,155 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>QEXTRCT</t>
+          <t>QHISPC</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7518642484417047</v>
+        <v>0.8803370950973293</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1080633726986945</v>
+        <v>0.1202941227691</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.184153634128851</v>
+        <v>-0.1034740134268362</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.04880562950779412</v>
+        <v>-0.2055870801357961</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02811185968668175</v>
+        <v>-0.1433395955485494</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>QEDLESHI</t>
+          <t>QNOHLTH</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8692554802113335</v>
+        <v>0.742742621222788</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2820098251129958</v>
+        <v>0.3825258295162977</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.09611805635391178</v>
+        <v>-0.09377154927699263</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.04435359362502852</v>
+        <v>-0.1242320407102496</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01766608572966158</v>
+        <v>0.1047037166043549</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>QNOHLTH</t>
+          <t>QESL</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7427426205749446</v>
+        <v>0.8669870467330312</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3825258292209991</v>
+        <v>0.1055887583105761</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.09377154783409625</v>
+        <v>-0.1218582076081707</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1242320404236909</v>
+        <v>-0.164540619176934</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1047037153226807</v>
+        <v>0.1246202491228288</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>QPOVTY</t>
+          <t>QEXTRCT</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4926703472929525</v>
+        <v>0.7518642472608691</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4936971001788416</v>
+        <v>0.1080633736403501</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01006171257136397</v>
+        <v>-0.1841536377102106</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.139980912263577</v>
+        <v>-0.04880562857143168</v>
       </c>
       <c r="F5" t="n">
-        <v>0.359303199780186</v>
+        <v>0.02811186015142211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>QESL</t>
+          <t>QEDLESHI</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8669870460373705</v>
+        <v>0.8692554803215153</v>
       </c>
       <c r="C6" t="n">
-        <v>0.105588759382269</v>
+        <v>0.2820098250435661</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1218582062889729</v>
+        <v>-0.09611805776404492</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1645406179565412</v>
+        <v>-0.04435359349460323</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1246202480462146</v>
+        <v>0.0176660870593831</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>QHISPC</t>
+          <t>PPUNIT</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8803370942915406</v>
+        <v>0.5203431762810202</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1202941229291331</v>
+        <v>0.1723556429544132</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.1034740124261152</v>
+        <v>-0.00853118410586568</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.205587078981756</v>
+        <v>-0.04118569700388107</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1433395948207157</v>
+        <v>-0.6351977639248791</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>PPUNIT</t>
+          <t>QPOVTY</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5203431752795143</v>
+        <v>0.4926703477871059</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1723556415683452</v>
+        <v>0.4936970987725287</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.008531183769641909</v>
+        <v>0.01006171317970551</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0411856994804425</v>
+        <v>-0.139980913852795</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.6351977636422353</v>
+        <v>0.3593032030497998</v>
       </c>
     </row>
     <row r="9">
@@ -741,217 +741,217 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1243576377146733</v>
+        <v>0.1243576388719362</v>
       </c>
       <c r="C9" t="n">
-        <v>0.66294007956358</v>
+        <v>0.6629400763354163</v>
       </c>
       <c r="D9" t="n">
-        <v>0.07601970061597395</v>
+        <v>0.0760197032434357</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.1184125638687395</v>
+        <v>-0.1184125657849894</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2379118979678956</v>
+        <v>0.2379118995421976</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>QFHH</t>
+          <t>QSERV</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2285252645071095</v>
+        <v>0.3709861022228685</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7131346566768045</v>
+        <v>0.5379072856593253</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2214646517180176</v>
+        <v>0.005759199727788074</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.07783278306666057</v>
+        <v>-0.08757769907133597</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.04601151712576505</v>
+        <v>0.155983972952657</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>QBLACK</t>
+          <t>QFHH</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.2749361517443922</v>
+        <v>0.2285252661260082</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7046485571608363</v>
+        <v>0.7131346559507746</v>
       </c>
       <c r="D11" t="n">
-        <v>0.05019711414732955</v>
+        <v>0.2214646558077026</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1307361802183043</v>
+        <v>-0.07783278425410714</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1670202047959224</v>
+        <v>-0.04601151511459178</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>QSERV</t>
+          <t>QBLACK</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3709861023078258</v>
+        <v>-0.2749361517979486</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5379072869833532</v>
+        <v>0.7046485575443674</v>
       </c>
       <c r="D12" t="n">
-        <v>0.005759199128988558</v>
+        <v>0.05019711505949858</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.08757769803385232</v>
+        <v>0.1307361815087761</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1559839714480021</v>
+        <v>0.1670202073710436</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>PERCAP</t>
+          <t>QRICH</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5037823282541694</v>
+        <v>0.4038778838595897</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7061433337952319</v>
+        <v>0.6463639855284391</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.04688443481784117</v>
+        <v>-0.06158261054806106</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1072480938194731</v>
+        <v>-0.1194534729670854</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.1020625141790412</v>
+        <v>0.002273121296869304</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>QRICH</t>
+          <t>PERCAP</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4038778847879076</v>
+        <v>0.5037823276587938</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6463639839109264</v>
+        <v>0.7061433370752405</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.06158260922857307</v>
+        <v>-0.04688443646465085</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.1194534731552246</v>
+        <v>-0.1072480927953808</v>
       </c>
       <c r="F14" t="n">
-        <v>0.002273121035538215</v>
+        <v>-0.1020625146575289</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>QRENTER</t>
+          <t>QNOAUTO</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1727227398097679</v>
+        <v>0.1891304089574793</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3584593755415023</v>
+        <v>0.3968119682334907</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.05642808994004768</v>
+        <v>-0.001312813755978878</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.4605499177939512</v>
+        <v>0.08291571045634666</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6579700024315055</v>
+        <v>0.5521493354761324</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>QNOAUTO</t>
+          <t>QRENTER</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.1891304089967761</v>
+        <v>0.1727227389210597</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3968119693850521</v>
+        <v>0.3584593742508944</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.001312813646046432</v>
+        <v>-0.05642809061090642</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0829157104879002</v>
+        <v>-0.46054991919618</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5521493306898304</v>
+        <v>0.6579699975112047</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>QFEMLBR</t>
+          <t>QFEMALE</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.4233895386433378</v>
+        <v>-0.1201784096346595</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2565876909270864</v>
+        <v>0.08442001695086726</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5549136206110808</v>
+        <v>0.9476420664224633</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.009510215744995571</v>
+        <v>0.01306748968427164</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.03382138915842849</v>
+        <v>-0.03709586659921296</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>QFEMALE</t>
+          <t>QFEMLBR</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.1201784102251344</v>
+        <v>-0.4233895389422812</v>
       </c>
       <c r="C18" t="n">
-        <v>0.08442001701203185</v>
+        <v>0.2565876914832129</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9476420859302027</v>
+        <v>0.5549136341195142</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01306748493548795</v>
+        <v>-0.009510221564061949</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.03709586765110615</v>
+        <v>-0.03382139079307862</v>
       </c>
     </row>
     <row r="19">
@@ -961,19 +961,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.1133192053356318</v>
+        <v>-0.1133192017874101</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.06739481110732691</v>
+        <v>-0.06739481440699845</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7290404171908992</v>
+        <v>0.729040421503802</v>
       </c>
       <c r="E19" t="n">
-        <v>0.4777003064674182</v>
+        <v>0.4777003061560329</v>
       </c>
       <c r="F19" t="n">
-        <v>0.06612983910678825</v>
+        <v>0.06612984087372405</v>
       </c>
     </row>
     <row r="20">
@@ -983,19 +983,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.3065470993356068</v>
+        <v>-0.3065470999719298</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.3702019246123122</v>
+        <v>-0.3702019232495327</v>
       </c>
       <c r="D20" t="n">
-        <v>0.04864970172662886</v>
+        <v>0.04864970237269507</v>
       </c>
       <c r="E20" t="n">
-        <v>0.6451312986528182</v>
+        <v>0.6451312943906372</v>
       </c>
       <c r="F20" t="n">
-        <v>0.09075704017158054</v>
+        <v>0.09075703803451746</v>
       </c>
     </row>
     <row r="21">
@@ -1005,19 +1005,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.08069646398190604</v>
+        <v>-0.08069646390827452</v>
       </c>
       <c r="C21" t="n">
-        <v>0.07089796134946129</v>
+        <v>0.0708979599700322</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1345297551567557</v>
+        <v>0.1345297566914315</v>
       </c>
       <c r="E21" t="n">
-        <v>0.8476251059191149</v>
+        <v>0.847625101158753</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.1136918292190382</v>
+        <v>-0.1136918263240227</v>
       </c>
     </row>
   </sheetData>
@@ -1129,19 +1129,19 @@
         <v>0.6695949908256502</v>
       </c>
       <c r="I2" t="n">
-        <v>4.983165035304014</v>
+        <v>4.983165037844279</v>
       </c>
       <c r="J2" t="n">
-        <v>3.692480325572514</v>
+        <v>3.692480322986977</v>
       </c>
       <c r="K2" t="n">
-        <v>1.902149211798767</v>
+        <v>1.902149201692064</v>
       </c>
       <c r="L2" t="n">
-        <v>1.763128716214867</v>
+        <v>1.763128705847649</v>
       </c>
       <c r="M2" t="n">
-        <v>1.467933697393225</v>
+        <v>1.467933700943554</v>
       </c>
     </row>
     <row r="3">
@@ -1172,19 +1172,19 @@
         <v>0.02479981447502408</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2491582517652007</v>
+        <v>0.249158251892214</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1846240162786257</v>
+        <v>0.1846240161493488</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09510746058993837</v>
+        <v>0.09510746008460322</v>
       </c>
       <c r="L3" t="n">
-        <v>0.08815643581074337</v>
+        <v>0.08815643529238243</v>
       </c>
       <c r="M3" t="n">
-        <v>0.07339668486966126</v>
+        <v>0.07339668504717768</v>
       </c>
     </row>
     <row r="4">
@@ -1215,19 +1215,19 @@
         <v>0.6087882918793165</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2491582517652007</v>
+        <v>0.249158251892214</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4337822680438264</v>
+        <v>0.4337822680415628</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5288897286337648</v>
+        <v>0.5288897281261661</v>
       </c>
       <c r="L4" t="n">
-        <v>0.6170461644445082</v>
+        <v>0.6170461634185485</v>
       </c>
       <c r="M4" t="n">
-        <v>0.6904428493141694</v>
+        <v>0.6904428484657261</v>
       </c>
     </row>
     <row r="5">
@@ -1258,19 +1258,19 @@
         <v>0.04073635253146473</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3608673071387364</v>
+        <v>0.3608673077661435</v>
       </c>
       <c r="J5" t="n">
-        <v>0.267399418303798</v>
+        <v>0.2673994184451512</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1377484909640392</v>
+        <v>0.1377484904014099</v>
       </c>
       <c r="L5" t="n">
-        <v>0.127681003428902</v>
+        <v>0.1276810028350356</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1063037801645243</v>
+        <v>0.1063037805522598</v>
       </c>
     </row>
   </sheetData>
@@ -1326,19 +1326,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.983165035304014</v>
+        <v>4.983165037844279</v>
       </c>
       <c r="C2" t="n">
-        <v>3.692480325572514</v>
+        <v>3.692480322986977</v>
       </c>
       <c r="D2" t="n">
-        <v>1.902149211798767</v>
+        <v>1.902149201692064</v>
       </c>
       <c r="E2" t="n">
-        <v>1.763128716214867</v>
+        <v>1.763128705847649</v>
       </c>
       <c r="F2" t="n">
-        <v>1.467933697393225</v>
+        <v>1.467933700943554</v>
       </c>
     </row>
     <row r="3">
@@ -1348,19 +1348,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2491582517652007</v>
+        <v>0.249158251892214</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1846240162786257</v>
+        <v>0.1846240161493488</v>
       </c>
       <c r="D3" t="n">
-        <v>0.09510746058993837</v>
+        <v>0.09510746008460322</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08815643581074337</v>
+        <v>0.08815643529238243</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07339668486966126</v>
+        <v>0.07339668504717768</v>
       </c>
     </row>
     <row r="4">
@@ -1370,19 +1370,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2491582517652007</v>
+        <v>0.249158251892214</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4337822680438264</v>
+        <v>0.4337822680415628</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5288897286337648</v>
+        <v>0.5288897281261661</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6170461644445082</v>
+        <v>0.6170461634185485</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6904428493141694</v>
+        <v>0.6904428484657261</v>
       </c>
     </row>
     <row r="5">
@@ -1392,19 +1392,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3608673071387364</v>
+        <v>0.3608673077661435</v>
       </c>
       <c r="C5" t="n">
-        <v>0.267399418303798</v>
+        <v>0.2673994184451512</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1377484909640392</v>
+        <v>0.1377484904014099</v>
       </c>
       <c r="E5" t="n">
-        <v>0.127681003428902</v>
+        <v>0.1276810028350356</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1063037801645243</v>
+        <v>0.1063037805522598</v>
       </c>
     </row>
   </sheetData>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[['QEXTRCT', 'QEDLESHI', 'QNOHLTH', 'QPOVTY', 'QESL', 'QHISPC', 'PPUNIT', 'PERCAP', 'QFAM', 'QFHH', 'QBLACK', 'QSERV', 'QRICH', 'QFEMLBR', 'QFEMALE', 'QAGEDEP', 'QRENTER', 'MEDAGE', 'QSSBEN', 'QNOAUTO']]</t>
+          <t>[['QHISPC', 'QNOHLTH', 'QESL', 'QEXTRCT', 'QEDLESHI', 'PPUNIT', 'QPOVTY', 'PERCAP', 'QFAM', 'QSERV', 'QFHH', 'QBLACK', 'QRICH', 'QFEMALE', 'QFEMLBR', 'QAGEDEP', 'QRENTER', 'MEDAGE', 'QSSBEN', 'QNOAUTO']]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">

</xml_diff>